<commit_message>
added ui extended benefits and rental assistance
</commit_message>
<xml_diff>
--- a/inst/extdata/economic_statistics.xlsx
+++ b/inst/extdata/economic_statistics.xlsx
@@ -5727,13 +5727,13 @@
         <v>1</v>
       </c>
       <c r="F206">
-        <v>4977.666666666667</v>
+        <v>4976.666666666667</v>
       </c>
       <c r="G206">
-        <v>13670.66666666667</v>
+        <v>13671.33333333333</v>
       </c>
       <c r="H206">
-        <v>323195.6666666667</v>
+        <v>323711.6666666667</v>
       </c>
     </row>
     <row r="207">
@@ -5753,13 +5753,13 @@
         <v>1</v>
       </c>
       <c r="F207">
-        <v>4983.111111111111</v>
+        <v>4982.777777777777</v>
       </c>
       <c r="G207">
-        <v>13687.55555555556</v>
+        <v>13687.77777777778</v>
       </c>
       <c r="H207">
-        <v>323319.2222222223</v>
+        <v>323491.2222222223</v>
       </c>
     </row>
     <row r="208">
@@ -5779,13 +5779,13 @@
         <v>1</v>
       </c>
       <c r="F208">
-        <v>4965.37037037037</v>
+        <v>4964.925925925926</v>
       </c>
       <c r="G208">
-        <v>13671.18518518518</v>
+        <v>13671.48148148148</v>
       </c>
       <c r="H208">
-        <v>324762.8518518519</v>
+        <v>324992.1851851852</v>
       </c>
     </row>
     <row r="209">
@@ -5805,13 +5805,13 @@
         <v>1</v>
       </c>
       <c r="F209">
-        <v>4975.382716049383</v>
+        <v>4974.79012345679</v>
       </c>
       <c r="G209">
-        <v>13676.46913580247</v>
+        <v>13676.86419753086</v>
       </c>
       <c r="H209">
-        <v>323759.2469135803</v>
+        <v>324065.024691358</v>
       </c>
     </row>
     <row r="210">
@@ -5831,13 +5831,13 @@
         <v>1</v>
       </c>
       <c r="F210">
-        <v>4974.621399176955</v>
+        <v>4974.164609053498</v>
       </c>
       <c r="G210">
-        <v>13678.40329218107</v>
+        <v>13678.70781893004</v>
       </c>
       <c r="H210">
-        <v>323947.1069958848</v>
+        <v>324182.8106995885</v>
       </c>
     </row>
     <row r="211">
@@ -5857,13 +5857,13 @@
         <v>1</v>
       </c>
       <c r="F211">
-        <v>4971.791495198902</v>
+        <v>4971.293552812072</v>
       </c>
       <c r="G211">
-        <v>13675.35253772291</v>
+        <v>13675.68449931413</v>
       </c>
       <c r="H211">
-        <v>324156.401920439</v>
+        <v>324413.3401920439</v>
       </c>
     </row>
     <row r="212">
@@ -5883,13 +5883,13 @@
         <v>1</v>
       </c>
       <c r="F212">
-        <v>4973.931870141747</v>
+        <v>4973.416095107453</v>
       </c>
       <c r="G212">
-        <v>13676.74165523548</v>
+        <v>13677.08550525835</v>
       </c>
       <c r="H212">
-        <v>323954.2519433014</v>
+        <v>324220.3918609968</v>
       </c>
     </row>
     <row r="213">
@@ -5909,13 +5909,13 @@
         <v>1</v>
       </c>
       <c r="F213">
-        <v>4973.448254839202</v>
+        <v>4972.958085657674</v>
       </c>
       <c r="G213">
-        <v>13676.83249504649</v>
+        <v>13677.15927450084</v>
       </c>
       <c r="H213">
-        <v>324019.2536198751</v>
+        <v>324272.1809175431</v>
       </c>
     </row>
     <row r="214">
@@ -5935,13 +5935,13 @@
         <v>1</v>
       </c>
       <c r="F214">
-        <v>4973.057206726617</v>
+        <v>4972.555911192399</v>
       </c>
       <c r="G214">
-        <v>13676.30889600163</v>
+        <v>13676.64309302444</v>
       </c>
       <c r="H214">
-        <v>324043.3024945385</v>
+        <v>324301.9709901946</v>
       </c>
     </row>
     <row r="215">
@@ -5961,13 +5961,13 @@
         <v>1</v>
       </c>
       <c r="F215">
-        <v>4973.479110569188</v>
+        <v>4972.976697319175</v>
       </c>
       <c r="G215">
-        <v>13676.62768209453</v>
+        <v>13676.96262426121</v>
       </c>
       <c r="H215">
-        <v>324005.602685905</v>
+        <v>324264.8479229115</v>
       </c>
     </row>
     <row r="216">
@@ -5987,13 +5987,13 @@
         <v>1</v>
       </c>
       <c r="F216">
-        <v>4973.328190711669</v>
+        <v>4972.830231389749</v>
       </c>
       <c r="G216">
-        <v>13676.58969104755</v>
+        <v>13676.92166392883</v>
       </c>
       <c r="H216">
-        <v>324022.7196001062</v>
+        <v>324279.6666102164</v>
       </c>
     </row>
     <row r="217">
@@ -6013,13 +6013,13 @@
         <v>1</v>
       </c>
       <c r="F217">
-        <v>4973.288169335825</v>
+        <v>4972.787613300441</v>
       </c>
       <c r="G217">
-        <v>13676.50875638123</v>
+        <v>13676.84246040482</v>
       </c>
       <c r="H217">
-        <v>324023.8749268499</v>
+        <v>324282.1618411075</v>
       </c>
     </row>
     <row r="218">
@@ -6039,13 +6039,13 @@
         <v>1</v>
       </c>
       <c r="F218">
-        <v>4973.365156872227</v>
+        <v>4972.864847336456</v>
       </c>
       <c r="G218">
-        <v>13676.57537650777</v>
+        <v>13676.90891619829</v>
       </c>
       <c r="H218">
-        <v>324017.3990709537</v>
+        <v>324275.5587914118</v>
       </c>
     </row>
     <row r="219">
@@ -6065,13 +6065,13 @@
         <v>1</v>
       </c>
       <c r="F219">
-        <v>4973.327172306574</v>
+        <v>4972.827564008882</v>
       </c>
       <c r="G219">
-        <v>13676.55794131218</v>
+        <v>13676.89101351065</v>
       </c>
       <c r="H219">
-        <v>324021.3311993032</v>
+        <v>324279.1290809119</v>
       </c>
     </row>
     <row r="220">
@@ -6091,13 +6091,13 @@
         <v>1</v>
       </c>
       <c r="F220">
-        <v>4973.326832838208</v>
+        <v>4972.826674881926</v>
       </c>
       <c r="G220">
-        <v>13676.54735806706</v>
+        <v>13676.88079670459</v>
       </c>
       <c r="H220">
-        <v>324020.8683990356</v>
+        <v>324278.9499044771</v>
       </c>
     </row>
     <row r="221">
@@ -6117,13 +6117,13 @@
         <v>1</v>
       </c>
       <c r="F221">
-        <v>4973.339720672337</v>
+        <v>4972.839695409088</v>
       </c>
       <c r="G221">
-        <v>13676.56022529567</v>
+        <v>13676.89357547117</v>
       </c>
       <c r="H221">
-        <v>324019.8662230975</v>
+        <v>324277.8792589336</v>
       </c>
     </row>
     <row r="222">
@@ -6143,13 +6143,13 @@
         <v>1</v>
       </c>
       <c r="F222">
-        <v>4973.33124193904</v>
+        <v>4972.831311433299</v>
       </c>
       <c r="G222">
-        <v>13676.55517489164</v>
+        <v>13676.88846189547</v>
       </c>
       <c r="H222">
-        <v>324020.6886071455</v>
+        <v>324278.6527481075</v>
       </c>
     </row>
     <row r="223">
@@ -6169,13 +6169,13 @@
         <v>1</v>
       </c>
       <c r="F223">
-        <v>4973.332598483195</v>
+        <v>4972.832560574771</v>
       </c>
       <c r="G223">
-        <v>13676.55425275146</v>
+        <v>13676.88761135708</v>
       </c>
       <c r="H223">
-        <v>324020.4744097595</v>
+        <v>324278.4939705061</v>
       </c>
     </row>
     <row r="224">
@@ -6195,13 +6195,13 @@
         <v>1</v>
       </c>
       <c r="F224">
-        <v>4973.334520364857</v>
+        <v>4972.834522472385</v>
       </c>
       <c r="G224">
-        <v>13676.55655097959</v>
+        <v>13676.8898829079</v>
       </c>
       <c r="H224">
-        <v>324020.3430800008</v>
+        <v>324278.3419925157</v>
       </c>
     </row>
     <row r="225">
@@ -6221,13 +6221,13 @@
         <v>1</v>
       </c>
       <c r="F225">
-        <v>4973.332786929031</v>
+        <v>4972.832798160152</v>
       </c>
       <c r="G225">
-        <v>13676.55532620756</v>
+        <v>13676.88865205348</v>
       </c>
       <c r="H225">
-        <v>324020.5020323019</v>
+        <v>324278.4962370431</v>
       </c>
     </row>
     <row r="226">
@@ -6247,13 +6247,13 @@
         <v>1</v>
       </c>
       <c r="F226">
-        <v>4973.333301925694</v>
+        <v>4972.833293735769</v>
       </c>
       <c r="G226">
-        <v>13676.5553766462</v>
+        <v>13676.88871543949</v>
       </c>
       <c r="H226">
-        <v>324020.4398406874</v>
+        <v>324278.4440666883</v>
       </c>
     </row>
     <row r="227">
@@ -6273,13 +6273,13 @@
         <v>1</v>
       </c>
       <c r="F227">
-        <v>4973.333536406527</v>
+        <v>4972.833538122769</v>
       </c>
       <c r="G227">
-        <v>13676.55575127778</v>
+        <v>13676.88908346696</v>
       </c>
       <c r="H227">
-        <v>324020.4283176634</v>
+        <v>324278.4274320824</v>
       </c>
     </row>
     <row r="228">
@@ -6299,13 +6299,13 @@
         <v>1</v>
       </c>
       <c r="F228">
-        <v>4973.333208420418</v>
+        <v>4972.83321000623</v>
       </c>
       <c r="G228">
-        <v>13676.55548471052</v>
+        <v>13676.88881698664</v>
       </c>
       <c r="H228">
-        <v>324020.4567302176</v>
+        <v>324278.4559119379</v>
       </c>
     </row>
     <row r="229">
@@ -6325,13 +6325,13 @@
         <v>1</v>
       </c>
       <c r="F229">
-        <v>4973.333348917547</v>
+        <v>4972.833347288256</v>
       </c>
       <c r="G229">
-        <v>13676.55553754483</v>
+        <v>13676.88887196436</v>
       </c>
       <c r="H229">
-        <v>324020.4416295228</v>
+        <v>324278.4424702362</v>
       </c>
     </row>
     <row r="230">
@@ -6351,13 +6351,13 @@
         <v>1</v>
       </c>
       <c r="F230">
-        <v>4973.333364581497</v>
+        <v>4972.833365139085</v>
       </c>
       <c r="G230">
-        <v>13676.55559117771</v>
+        <v>13676.88892413932</v>
       </c>
       <c r="H230">
-        <v>324020.4422258012</v>
+        <v>324278.4419380855</v>
       </c>
     </row>
     <row r="231">
@@ -6377,13 +6377,13 @@
         <v>1</v>
       </c>
       <c r="F231">
-        <v>4973.333307306487</v>
+        <v>4972.833307477857</v>
       </c>
       <c r="G231">
-        <v>13676.55553781102</v>
+        <v>13676.88887103011</v>
       </c>
       <c r="H231">
-        <v>324020.4468618472</v>
+        <v>324278.4467734199</v>
       </c>
     </row>
     <row r="232">
@@ -6403,13 +6403,13 @@
         <v>1</v>
       </c>
       <c r="F232">
-        <v>4973.33334026851</v>
+        <v>4972.833339968399</v>
       </c>
       <c r="G232">
-        <v>13676.55555551119</v>
+        <v>13676.8888890446</v>
       </c>
       <c r="H232">
-        <v>324020.4435723904</v>
+        <v>324278.4437272472</v>
       </c>
     </row>
     <row r="233">
@@ -6429,13 +6429,13 @@
         <v>1</v>
       </c>
       <c r="F233">
-        <v>4973.333337385499</v>
+        <v>4972.833337528447</v>
       </c>
       <c r="G233">
-        <v>13676.55556149997</v>
+        <v>13676.88889473801</v>
       </c>
       <c r="H233">
-        <v>324020.4442200129</v>
+        <v>324278.4441462508</v>
       </c>
     </row>
     <row r="234">
@@ -6455,13 +6455,13 @@
         <v>1</v>
       </c>
       <c r="F234">
-        <v>4973.333328320166</v>
+        <v>4972.8333283249</v>
       </c>
       <c r="G234">
-        <v>13676.55555160739</v>
+        <v>13676.88888493757</v>
       </c>
       <c r="H234">
-        <v>324020.4448847502</v>
+        <v>324278.444882306</v>
       </c>
     </row>
     <row r="235">
@@ -6481,13 +6481,13 @@
         <v>1</v>
       </c>
       <c r="F235">
-        <v>4973.333335324724</v>
+        <v>4972.833335273916</v>
       </c>
       <c r="G235">
-        <v>13676.55555620618</v>
+        <v>13676.88888957339</v>
       </c>
       <c r="H235">
-        <v>324020.4442257179</v>
+        <v>324278.4442519347</v>
       </c>
     </row>
     <row r="236">
@@ -6507,13 +6507,13 @@
         <v>1</v>
       </c>
       <c r="F236">
-        <v>4973.333333676796</v>
+        <v>4972.833333709087</v>
       </c>
       <c r="G236">
-        <v>13676.55555643785</v>
+        <v>13676.88888974966</v>
       </c>
       <c r="H236">
-        <v>324020.4444434937</v>
+        <v>324278.4444268305</v>
       </c>
     </row>
     <row r="237">
@@ -6533,13 +6533,13 @@
         <v>1</v>
       </c>
       <c r="F237">
-        <v>4973.333332440562</v>
+        <v>4972.833332435967</v>
       </c>
       <c r="G237">
-        <v>13676.55555475048</v>
+        <v>13676.88888808687</v>
       </c>
       <c r="H237">
-        <v>324020.4445179873</v>
+        <v>324278.4445203571</v>
       </c>
     </row>
     <row r="238">
@@ -6559,13 +6559,13 @@
         <v>1</v>
       </c>
       <c r="F238">
-        <v>4973.333333814027</v>
+        <v>4972.833333806323</v>
       </c>
       <c r="G238">
-        <v>13676.55555579817</v>
+        <v>13676.88888913664</v>
       </c>
       <c r="H238">
-        <v>324020.444395733</v>
+        <v>324278.4443997074</v>
       </c>
     </row>
     <row r="239">
@@ -6585,13 +6585,13 @@
         <v>1</v>
       </c>
       <c r="F239">
-        <v>4973.333333310462</v>
+        <v>4972.833333317126</v>
       </c>
       <c r="G239">
-        <v>13676.55555566217</v>
+        <v>13676.88888899106</v>
       </c>
       <c r="H239">
-        <v>324020.4444524046</v>
+        <v>324278.444448965</v>
       </c>
     </row>
     <row r="240">
@@ -6611,13 +6611,13 @@
         <v>1</v>
       </c>
       <c r="F240">
-        <v>4973.333333188351</v>
+        <v>4972.833333186472</v>
       </c>
       <c r="G240">
-        <v>13676.5555554036</v>
+        <v>13676.88888873819</v>
       </c>
       <c r="H240">
-        <v>324020.444455375</v>
+        <v>324278.4444563432</v>
       </c>
     </row>
     <row r="241">
@@ -6637,13 +6637,13 @@
         <v>1</v>
       </c>
       <c r="F241">
-        <v>4973.333333437613</v>
+        <v>4972.833333436641</v>
       </c>
       <c r="G241">
-        <v>13676.55555562131</v>
+        <v>13676.8888889553</v>
       </c>
       <c r="H241">
-        <v>324020.4444345042</v>
+        <v>324278.4444350052</v>
       </c>
     </row>
     <row r="242">
@@ -6663,13 +6663,13 @@
         <v>1</v>
       </c>
       <c r="F242">
-        <v>4973.333333312142</v>
+        <v>4972.833333313413</v>
       </c>
       <c r="G242">
-        <v>13676.55555556236</v>
+        <v>13676.88888889485</v>
       </c>
       <c r="H242">
-        <v>324020.4444474279</v>
+        <v>324278.4444467711</v>
       </c>
     </row>
     <row r="243">
@@ -6689,13 +6689,13 @@
         <v>1</v>
       </c>
       <c r="F243">
-        <v>4973.333333312702</v>
+        <v>4972.833333312176</v>
       </c>
       <c r="G243">
-        <v>13676.55555552909</v>
+        <v>13676.88888886278</v>
       </c>
       <c r="H243">
-        <v>324020.444445769</v>
+        <v>324278.4444460399</v>
       </c>
     </row>
     <row r="244">
@@ -6715,13 +6715,13 @@
         <v>1</v>
       </c>
       <c r="F244">
-        <v>4973.333333354152</v>
+        <v>4972.833333354077</v>
       </c>
       <c r="G244">
-        <v>13676.55555557092</v>
+        <v>13676.88888890431</v>
       </c>
       <c r="H244">
-        <v>324020.4444425671</v>
+        <v>324278.4444426054</v>
       </c>
     </row>
     <row r="245">
@@ -6741,13 +6741,13 @@
         <v>1</v>
       </c>
       <c r="F245">
-        <v>4973.333333326332</v>
+        <v>4972.833333326556</v>
       </c>
       <c r="G245">
-        <v>13676.55555555413</v>
+        <v>13676.88888888731</v>
       </c>
       <c r="H245">
-        <v>324020.4444452547</v>
+        <v>324278.4444451388</v>
       </c>
     </row>
     <row r="246">
@@ -6767,13 +6767,13 @@
         <v>1</v>
       </c>
       <c r="F246">
-        <v>4973.333333331062</v>
+        <v>4972.833333330936</v>
       </c>
       <c r="G246">
-        <v>13676.55555555138</v>
+        <v>13676.8888888848</v>
       </c>
       <c r="H246">
-        <v>324020.4444445302</v>
+        <v>324278.4444445947</v>
       </c>
     </row>
     <row r="247">
@@ -6793,13 +6793,13 @@
         <v>1</v>
       </c>
       <c r="F247">
-        <v>4973.333333337182</v>
+        <v>4972.833333337189</v>
       </c>
       <c r="G247">
-        <v>13676.55555555881</v>
+        <v>13676.88888889214</v>
       </c>
       <c r="H247">
-        <v>324020.4444441173</v>
+        <v>324278.444444113</v>
       </c>
     </row>
     <row r="248">
@@ -6819,13 +6819,13 @@
         <v>1</v>
       </c>
       <c r="F248">
-        <v>4973.333333331525</v>
+        <v>4972.83333333156</v>
       </c>
       <c r="G248">
-        <v>13676.55555555477</v>
+        <v>13676.88888888808</v>
       </c>
       <c r="H248">
-        <v>324020.4444446341</v>
+        <v>324278.4444446155</v>
       </c>
     </row>
     <row r="249">
@@ -6845,13 +6845,13 @@
         <v>1</v>
       </c>
       <c r="F249">
-        <v>4973.333333333257</v>
+        <v>4972.833333333228</v>
       </c>
       <c r="G249">
-        <v>13676.55555555499</v>
+        <v>13676.88888888834</v>
       </c>
       <c r="H249">
-        <v>324020.4444444272</v>
+        <v>324278.444444441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>